<commit_message>
Helper methods to fix inputs created inside of InputHandler. SearchAndSave now goes through FastPeopleSearch and finds numbers and mailing addresses of those people. Person was created to organize the information of each search for an easy output.
</commit_message>
<xml_diff>
--- a/2 26 19 Skip Tracing.xlsx
+++ b/2 26 19 Skip Tracing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rimes\OneDrive\Desktop\Python Practice\WholeSaleScrapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ddf82aa752a6d42/Desktop/Python Practice/WholeSaleScrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39901891-284B-4239-9B8D-FC0D2444017A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:AG1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>